<commit_message>
Updated Tableplan.ods and dsa-4.1.xlsx
</commit_message>
<xml_diff>
--- a/src/site/documents/rulesets/dsa-4.1/dsa-4.1.xlsx
+++ b/src/site/documents/rulesets/dsa-4.1/dsa-4.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gianni\Documents\Java Programme\Goetterblick\src\site\documents\rulesets\dsa-4.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D01EDA-5046-4E51-BD7E-2FAF6BC6D788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C599A45-1343-455E-870D-2EB49D9B118A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Eigenschaften" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2419" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2449" uniqueCount="402">
   <si>
     <t>tid</t>
   </si>
@@ -1046,9 +1046,6 @@
     <t>weight_subtr</t>
   </si>
   <si>
-    <t>age_calc</t>
-  </si>
-  <si>
     <t>mittelland</t>
   </si>
   <si>
@@ -1061,21 +1058,6 @@
     <t>zwerge</t>
   </si>
   <si>
-    <t>elfen</t>
-  </si>
-  <si>
-    <t>halbelfen</t>
-  </si>
-  <si>
-    <t>15+1d3</t>
-  </si>
-  <si>
-    <t>35+1d6</t>
-  </si>
-  <si>
-    <t>25+1d20</t>
-  </si>
-  <si>
     <t>hex_code</t>
   </si>
   <si>
@@ -1185,6 +1167,90 @@
   </si>
   <si>
     <t>dark-purple</t>
+  </si>
+  <si>
+    <t>nivese</t>
+  </si>
+  <si>
+    <t>norbarden</t>
+  </si>
+  <si>
+    <t>trollzacker</t>
+  </si>
+  <si>
+    <t>waldmenschen</t>
+  </si>
+  <si>
+    <t>utulus</t>
+  </si>
+  <si>
+    <t>rochshaz</t>
+  </si>
+  <si>
+    <t>tocamuyac</t>
+  </si>
+  <si>
+    <t>auelfen</t>
+  </si>
+  <si>
+    <t>waldelfen</t>
+  </si>
+  <si>
+    <t>firnelfen</t>
+  </si>
+  <si>
+    <t>halbelfen-auelf</t>
+  </si>
+  <si>
+    <t>halbelfen-firnelf</t>
+  </si>
+  <si>
+    <t>halbelfen-thorwalisch</t>
+  </si>
+  <si>
+    <t>halbelfen-nivesisch</t>
+  </si>
+  <si>
+    <t>brilliantzwerge</t>
+  </si>
+  <si>
+    <t>amboszwerge</t>
+  </si>
+  <si>
+    <t>wilde-zwerge</t>
+  </si>
+  <si>
+    <t>orkfrau</t>
+  </si>
+  <si>
+    <t>halborks</t>
+  </si>
+  <si>
+    <t>orks</t>
+  </si>
+  <si>
+    <t>goblins</t>
+  </si>
+  <si>
+    <t>goblinfrau</t>
+  </si>
+  <si>
+    <t>achaz</t>
+  </si>
+  <si>
+    <t>orkland-achaz</t>
+  </si>
+  <si>
+    <t>maraskan-achaz</t>
+  </si>
+  <si>
+    <t>erzzwerge</t>
+  </si>
+  <si>
+    <t>age_min</t>
+  </si>
+  <si>
+    <t>age_max</t>
   </si>
 </sst>
 </file>
@@ -1715,10 +1781,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C126EB39-5F8A-4A17-AC04-D6314E24D7EA}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1732,16 +1798,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1749,7 +1815,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -1763,7 +1829,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
@@ -1777,7 +1843,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="C4" s="2">
         <v>10</v>
@@ -1791,7 +1857,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="C5" s="2">
         <v>12</v>
@@ -1805,7 +1871,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="C6" s="2">
         <v>18</v>
@@ -1819,7 +1885,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="C7" s="2">
         <v>20</v>
@@ -1833,7 +1899,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
@@ -1847,7 +1913,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="C9" s="2">
         <v>5</v>
@@ -1861,7 +1927,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="C10" s="2">
         <v>13</v>
@@ -1875,7 +1941,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="C11" s="2">
         <v>17</v>
@@ -1889,7 +1955,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="C12" s="2">
         <v>19</v>
@@ -1903,7 +1969,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="C13" s="2">
         <v>20</v>
@@ -1917,7 +1983,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="C14" s="2">
         <v>1</v>
@@ -1931,7 +1997,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="C15" s="2">
         <v>3</v>
@@ -1945,7 +2011,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="C16" s="2">
         <v>8</v>
@@ -1959,7 +2025,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="C17" s="2">
         <v>12</v>
@@ -1973,7 +2039,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="C18" s="2">
         <v>19</v>
@@ -1987,7 +2053,7 @@
         <v>3</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="C19" s="2">
         <v>1</v>
@@ -2001,7 +2067,7 @@
         <v>3</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="C20" s="2">
         <v>3</v>
@@ -2015,7 +2081,7 @@
         <v>3</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="C21" s="2">
         <v>6</v>
@@ -2029,7 +2095,7 @@
         <v>3</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="C22" s="2">
         <v>10</v>
@@ -2043,7 +2109,7 @@
         <v>3</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="C23" s="2">
         <v>11</v>
@@ -2057,7 +2123,7 @@
         <v>3</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="C24" s="2">
         <v>15</v>
@@ -2071,7 +2137,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="C25" s="2">
         <v>1</v>
@@ -2085,7 +2151,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="C26" s="2">
         <v>3</v>
@@ -2099,7 +2165,7 @@
         <v>4</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="C27" s="2">
         <v>5</v>
@@ -2113,7 +2179,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="C28" s="2">
         <v>9</v>
@@ -2127,7 +2193,7 @@
         <v>4</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="C29" s="2">
         <v>13</v>
@@ -2141,7 +2207,7 @@
         <v>4</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="C30" s="2">
         <v>17</v>
@@ -2155,7 +2221,7 @@
         <v>4</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="C31" s="2">
         <v>19</v>
@@ -2169,7 +2235,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="C32" s="2">
         <v>20</v>
@@ -2183,7 +2249,7 @@
         <v>5</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="C33" s="2">
         <v>1</v>
@@ -2197,7 +2263,7 @@
         <v>5</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="C34" s="2">
         <v>4</v>
@@ -2211,7 +2277,7 @@
         <v>5</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="C35" s="2">
         <v>7</v>
@@ -2225,7 +2291,7 @@
         <v>5</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="C36" s="2">
         <v>11</v>
@@ -2239,7 +2305,7 @@
         <v>5</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="C37" s="2">
         <v>15</v>
@@ -2253,7 +2319,7 @@
         <v>5</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="C38" s="2">
         <v>17</v>
@@ -2267,7 +2333,7 @@
         <v>5</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="C39" s="2">
         <v>19</v>
@@ -2281,12 +2347,96 @@
         <v>5</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="C40" s="2">
         <v>20</v>
       </c>
       <c r="D40" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>6</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="C41" s="2">
+        <v>1</v>
+      </c>
+      <c r="D41" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>6</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C42" s="2">
+        <v>3</v>
+      </c>
+      <c r="D42" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>6</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="C43" s="2">
+        <v>10</v>
+      </c>
+      <c r="D43" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>6</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="C44" s="2">
+        <v>15</v>
+      </c>
+      <c r="D44" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>6</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="C45" s="2">
+        <v>18</v>
+      </c>
+      <c r="D45" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>6</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C46" s="2">
+        <v>20</v>
+      </c>
+      <c r="D46" s="2">
         <v>20</v>
       </c>
     </row>
@@ -11729,7 +11879,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11927,7 +12077,7 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11954,7 +12104,7 @@
         <v>47</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -11968,7 +12118,7 @@
         <v>31</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -11982,7 +12132,7 @@
         <v>31</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -11996,7 +12146,7 @@
         <v>31</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -12010,7 +12160,7 @@
         <v>31</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -12024,7 +12174,7 @@
         <v>31</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -12038,7 +12188,7 @@
         <v>31</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -12052,7 +12202,7 @@
         <v>31</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -12066,7 +12216,7 @@
         <v>31</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -12080,7 +12230,7 @@
         <v>31</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -12094,7 +12244,7 @@
         <v>31</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -12108,7 +12258,7 @@
         <v>31</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -12122,7 +12272,7 @@
         <v>31</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -12136,7 +12286,7 @@
         <v>31</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -12150,7 +12300,7 @@
         <v>31</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -12164,7 +12314,7 @@
         <v>31</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -12178,7 +12328,7 @@
         <v>31</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -12192,7 +12342,7 @@
         <v>31</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -12206,7 +12356,7 @@
         <v>31</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -12220,7 +12370,7 @@
         <v>31</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -12234,7 +12384,7 @@
         <v>31</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -12577,7 +12727,7 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12604,7 +12754,7 @@
         <v>47</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -12618,7 +12768,7 @@
         <v>31</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -12632,7 +12782,7 @@
         <v>31</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -12646,7 +12796,7 @@
         <v>31</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -12660,7 +12810,7 @@
         <v>31</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -12674,7 +12824,7 @@
         <v>31</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -12688,7 +12838,7 @@
         <v>31</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -12702,7 +12852,7 @@
         <v>31</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -12716,7 +12866,7 @@
         <v>31</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -12730,7 +12880,7 @@
         <v>31</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -12744,7 +12894,7 @@
         <v>31</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -12758,7 +12908,7 @@
         <v>31</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -12772,7 +12922,7 @@
         <v>31</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -12786,7 +12936,7 @@
         <v>31</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -12800,7 +12950,7 @@
         <v>31</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -12814,7 +12964,7 @@
         <v>31</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -13209,10 +13359,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EF64AA8-8A48-4D17-8607-268D13AA7A05}">
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13220,18 +13370,19 @@
     <col min="1" max="1" width="3.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="11.42578125" style="2"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -13260,27 +13411,27 @@
         <v>332</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>333</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
@@ -13294,14 +13445,17 @@
       <c r="I2" s="2">
         <v>100</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>340</v>
+      <c r="J2" s="2">
+        <v>16</v>
       </c>
       <c r="K2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -13312,10 +13466,7 @@
         <v>31</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0</v>
+        <v>334</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
@@ -13329,14 +13480,17 @@
       <c r="I3" s="2">
         <v>105</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>340</v>
+      <c r="J3" s="2">
+        <v>16</v>
       </c>
       <c r="K3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -13347,10 +13501,7 @@
         <v>31</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0</v>
+        <v>335</v>
       </c>
       <c r="F4" s="2">
         <v>5</v>
@@ -13364,14 +13515,17 @@
       <c r="I4" s="2">
         <v>95</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>340</v>
+      <c r="J4" s="2">
+        <v>16</v>
       </c>
       <c r="K4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -13382,10 +13536,7 @@
         <v>31</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="E5" s="2">
-        <v>1</v>
+        <v>336</v>
       </c>
       <c r="F5" s="2">
         <v>16</v>
@@ -13399,14 +13550,17 @@
       <c r="I5" s="2">
         <v>80</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>341</v>
+      <c r="J5" s="2">
+        <v>36</v>
       </c>
       <c r="K5" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -13417,10 +13571,7 @@
         <v>31</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="E6" s="2">
-        <v>2</v>
+        <v>381</v>
       </c>
       <c r="F6" s="2">
         <v>20</v>
@@ -13434,14 +13585,17 @@
       <c r="I6" s="2">
         <v>120</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>342</v>
+      <c r="J6" s="2">
+        <v>26</v>
       </c>
       <c r="K6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -13452,10 +13606,7 @@
         <v>31</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="E7" s="2">
-        <v>3</v>
+        <v>384</v>
       </c>
       <c r="F7" s="2">
         <v>3</v>
@@ -13469,14 +13620,17 @@
       <c r="I7" s="2">
         <v>120</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>340</v>
+      <c r="J7" s="2">
+        <v>16</v>
       </c>
       <c r="K7" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -13486,8 +13640,32 @@
       <c r="C8" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D8" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="F8" s="2">
+        <v>4</v>
+      </c>
+      <c r="G8" s="2">
+        <v>157</v>
+      </c>
+      <c r="H8" s="2">
+        <v>195</v>
+      </c>
+      <c r="I8" s="2">
+        <v>110</v>
+      </c>
+      <c r="J8" s="2">
+        <v>15</v>
+      </c>
+      <c r="K8" s="2">
+        <v>17</v>
+      </c>
+      <c r="L8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -13497,8 +13675,23 @@
       <c r="C9" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D9" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="F9" s="2">
+        <v>3</v>
+      </c>
+      <c r="J9" s="2">
+        <v>16</v>
+      </c>
+      <c r="K9" s="2">
+        <v>18</v>
+      </c>
+      <c r="L9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -13508,8 +13701,23 @@
       <c r="C10" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D10" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="F10" s="2">
+        <v>7</v>
+      </c>
+      <c r="J10" s="2">
+        <v>15</v>
+      </c>
+      <c r="K10" s="2">
+        <v>17</v>
+      </c>
+      <c r="L10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -13519,8 +13727,23 @@
       <c r="C11" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D11" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="F11" s="2">
+        <v>6</v>
+      </c>
+      <c r="J11" s="2">
+        <v>15</v>
+      </c>
+      <c r="K11" s="2">
+        <v>17</v>
+      </c>
+      <c r="L11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -13530,8 +13753,23 @@
       <c r="C12" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D12" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F12" s="2">
+        <v>5</v>
+      </c>
+      <c r="J12" s="2">
+        <v>15</v>
+      </c>
+      <c r="K12" s="2">
+        <v>17</v>
+      </c>
+      <c r="L12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -13541,8 +13779,23 @@
       <c r="C13" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D13" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="F13" s="2">
+        <v>3</v>
+      </c>
+      <c r="J13" s="2">
+        <v>15</v>
+      </c>
+      <c r="K13" s="2">
+        <v>17</v>
+      </c>
+      <c r="L13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -13552,8 +13805,23 @@
       <c r="C14" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D14" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="F14" s="2">
+        <v>9</v>
+      </c>
+      <c r="J14" s="2">
+        <v>15</v>
+      </c>
+      <c r="K14" s="2">
+        <v>17</v>
+      </c>
+      <c r="L14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -13563,8 +13831,23 @@
       <c r="C15" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D15" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="F15" s="2">
+        <v>23</v>
+      </c>
+      <c r="J15" s="2">
+        <v>26</v>
+      </c>
+      <c r="K15" s="2">
+        <v>45</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -13574,8 +13857,23 @@
       <c r="C16" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="F16" s="2">
+        <v>24</v>
+      </c>
+      <c r="J16" s="2">
+        <v>26</v>
+      </c>
+      <c r="K16" s="2">
+        <v>45</v>
+      </c>
+      <c r="L16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -13585,8 +13883,23 @@
       <c r="C17" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="F17" s="2">
+        <v>5</v>
+      </c>
+      <c r="J17" s="2">
+        <v>16</v>
+      </c>
+      <c r="K17" s="2">
+        <v>18</v>
+      </c>
+      <c r="L17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -13596,8 +13909,23 @@
       <c r="C18" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F18" s="2">
+        <v>8</v>
+      </c>
+      <c r="J18" s="2">
+        <v>16</v>
+      </c>
+      <c r="K18" s="2">
+        <v>18</v>
+      </c>
+      <c r="L18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -13607,8 +13935,23 @@
       <c r="C19" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="F19" s="2">
+        <v>4</v>
+      </c>
+      <c r="J19" s="2">
+        <v>16</v>
+      </c>
+      <c r="K19" s="2">
+        <v>18</v>
+      </c>
+      <c r="L19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -13618,8 +13961,23 @@
       <c r="C20" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="F20" s="2">
+        <v>12</v>
+      </c>
+      <c r="J20" s="2">
+        <v>36</v>
+      </c>
+      <c r="K20" s="2">
+        <v>41</v>
+      </c>
+      <c r="L20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -13629,8 +13987,23 @@
       <c r="C21" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="F21" s="2">
+        <v>12</v>
+      </c>
+      <c r="J21" s="2">
+        <v>36</v>
+      </c>
+      <c r="K21" s="2">
+        <v>41</v>
+      </c>
+      <c r="L21" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -13640,8 +14013,23 @@
       <c r="C22" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="F22" s="2">
+        <v>16</v>
+      </c>
+      <c r="J22" s="2">
+        <v>36</v>
+      </c>
+      <c r="K22" s="2">
+        <v>41</v>
+      </c>
+      <c r="L22" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -13651,8 +14039,23 @@
       <c r="C23" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="F23" s="2">
+        <v>16</v>
+      </c>
+      <c r="J23" s="2">
+        <v>36</v>
+      </c>
+      <c r="K23" s="2">
+        <v>41</v>
+      </c>
+      <c r="L23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -13662,8 +14065,23 @@
       <c r="C24" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="F24" s="2">
+        <v>12</v>
+      </c>
+      <c r="J24" s="2">
+        <v>13</v>
+      </c>
+      <c r="K24" s="2">
+        <v>15</v>
+      </c>
+      <c r="L24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -13673,8 +14091,23 @@
       <c r="C25" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="F25" s="2">
+        <v>2</v>
+      </c>
+      <c r="J25" s="2">
+        <v>13</v>
+      </c>
+      <c r="K25" s="2">
+        <v>15</v>
+      </c>
+      <c r="L25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -13684,8 +14117,23 @@
       <c r="C26" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="F26" s="2">
+        <v>1</v>
+      </c>
+      <c r="J26" s="2">
+        <v>14</v>
+      </c>
+      <c r="K26" s="2">
+        <v>16</v>
+      </c>
+      <c r="L26" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -13695,8 +14143,23 @@
       <c r="C27" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="F27" s="2">
+        <v>3</v>
+      </c>
+      <c r="J27" s="2">
+        <v>11</v>
+      </c>
+      <c r="K27" s="2">
+        <v>13</v>
+      </c>
+      <c r="L27" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>26</v>
       </c>
@@ -13706,8 +14169,23 @@
       <c r="C28" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="F28" s="2">
+        <v>7</v>
+      </c>
+      <c r="J28" s="2">
+        <v>11</v>
+      </c>
+      <c r="K28" s="2">
+        <v>13</v>
+      </c>
+      <c r="L28" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>27</v>
       </c>
@@ -13717,8 +14195,23 @@
       <c r="C29" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="F29" s="2">
+        <v>14</v>
+      </c>
+      <c r="J29" s="2">
+        <v>21</v>
+      </c>
+      <c r="K29" s="2">
+        <v>23</v>
+      </c>
+      <c r="L29" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>28</v>
       </c>
@@ -13728,8 +14221,23 @@
       <c r="C30" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="F30" s="2">
+        <v>9</v>
+      </c>
+      <c r="J30" s="2">
+        <v>21</v>
+      </c>
+      <c r="K30" s="2">
+        <v>23</v>
+      </c>
+      <c r="L30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>29</v>
       </c>
@@ -13739,8 +14247,23 @@
       <c r="C31" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="F31" s="2">
+        <v>16</v>
+      </c>
+      <c r="J31" s="2">
+        <v>21</v>
+      </c>
+      <c r="K31" s="2">
+        <v>23</v>
+      </c>
+      <c r="L31" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>30</v>
       </c>
@@ -13921,10 +14444,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6DE890F-0693-4D17-9600-9AF061C8B1DE}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13938,16 +14461,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -13955,7 +14478,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -13969,7 +14492,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="C3" s="2">
         <v>4</v>
@@ -13983,7 +14506,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="C4" s="2">
         <v>8</v>
@@ -13997,7 +14520,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="C5" s="2">
         <v>13</v>
@@ -14011,7 +14534,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="C6" s="2">
         <v>17</v>
@@ -14025,7 +14548,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="C7" s="2">
         <v>19</v>
@@ -14039,7 +14562,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
@@ -14053,7 +14576,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="C9" s="2">
         <v>7</v>
@@ -14067,7 +14590,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="C10" s="2">
         <v>13</v>
@@ -14081,7 +14604,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="C11" s="2">
         <v>15</v>
@@ -14095,7 +14618,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="C12" s="2">
         <v>18</v>
@@ -14109,7 +14632,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="C13" s="2">
         <v>20</v>
@@ -14123,7 +14646,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="C14" s="2">
         <v>1</v>
@@ -14137,7 +14660,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="C15" s="2">
         <v>9</v>
@@ -14151,7 +14674,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="C16" s="2">
         <v>14</v>
@@ -14165,7 +14688,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="C17" s="2">
         <v>16</v>
@@ -14179,7 +14702,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="C18" s="2">
         <v>18</v>
@@ -14193,7 +14716,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="C19" s="2">
         <v>19</v>
@@ -14207,7 +14730,7 @@
         <v>2</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="C20" s="2">
         <v>20</v>
@@ -14221,7 +14744,7 @@
         <v>3</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="C21" s="2">
         <v>1</v>
@@ -14235,7 +14758,7 @@
         <v>3</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="C22" s="2">
         <v>6</v>
@@ -14249,7 +14772,7 @@
         <v>3</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="C23" s="2">
         <v>10</v>
@@ -14263,7 +14786,7 @@
         <v>3</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="C24" s="2">
         <v>12</v>
@@ -14277,7 +14800,7 @@
         <v>3</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="C25" s="2">
         <v>14</v>
@@ -14291,7 +14814,7 @@
         <v>3</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="C26" s="2">
         <v>15</v>
@@ -14305,7 +14828,7 @@
         <v>3</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="C27" s="2">
         <v>16</v>
@@ -14319,7 +14842,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="C28" s="2">
         <v>18</v>
@@ -14333,7 +14856,7 @@
         <v>4</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="C29" s="2">
         <v>1</v>
@@ -14347,7 +14870,7 @@
         <v>4</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="C30" s="2">
         <v>2</v>
@@ -14361,7 +14884,7 @@
         <v>4</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="C31" s="2">
         <v>4</v>
@@ -14375,7 +14898,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="C32" s="2">
         <v>6</v>
@@ -14389,7 +14912,7 @@
         <v>4</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="C33" s="2">
         <v>8</v>
@@ -14403,7 +14926,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="C34" s="2">
         <v>12</v>
@@ -14417,7 +14940,7 @@
         <v>4</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="C35" s="2">
         <v>18</v>
@@ -14431,7 +14954,7 @@
         <v>5</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="C36" s="2">
         <v>1</v>
@@ -14445,7 +14968,7 @@
         <v>5</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="C37" s="2">
         <v>4</v>
@@ -14459,7 +14982,7 @@
         <v>5</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="C38" s="2">
         <v>7</v>
@@ -14473,7 +14996,7 @@
         <v>5</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="C39" s="2">
         <v>11</v>
@@ -14487,7 +15010,7 @@
         <v>5</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="C40" s="2">
         <v>16</v>
@@ -14501,7 +15024,7 @@
         <v>5</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="C41" s="2">
         <v>18</v>
@@ -14515,12 +15038,82 @@
         <v>5</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="C42" s="2">
         <v>20</v>
       </c>
       <c r="D42" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>6</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C43" s="2">
+        <v>1</v>
+      </c>
+      <c r="D43" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>6</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C44" s="2">
+        <v>16</v>
+      </c>
+      <c r="D44" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>6</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="C45" s="2">
+        <v>17</v>
+      </c>
+      <c r="D45" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>6</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="C46" s="2">
+        <v>19</v>
+      </c>
+      <c r="D46" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>6</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="C47" s="2">
+        <v>20</v>
+      </c>
+      <c r="D47" s="2">
         <v>20</v>
       </c>
     </row>

</xml_diff>